<commit_message>
cham cong & fix soft delete
</commit_message>
<xml_diff>
--- a/KeToanTienLuong/Resources/cham_cong_form.xlsx
+++ b/KeToanTienLuong/Resources/cham_cong_form.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Số</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Tiền thưởng</t>
+  </si>
+  <si>
+    <t>Tiền phạt</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,7 +440,7 @@
     <col min="7" max="7" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,8 +462,11 @@
       <c r="G1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -482,8 +488,11 @@
       <c r="G2">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -505,8 +514,11 @@
       <c r="G3">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -528,8 +540,11 @@
       <c r="G4">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -551,8 +566,11 @@
       <c r="G5">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -574,8 +592,11 @@
       <c r="G6">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -597,8 +618,11 @@
       <c r="G7">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -620,8 +644,11 @@
       <c r="G8">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -643,8 +670,11 @@
       <c r="G9">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -666,8 +696,11 @@
       <c r="G10">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -689,8 +722,11 @@
       <c r="G11">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -712,8 +748,11 @@
       <c r="G12">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -735,8 +774,11 @@
       <c r="G13">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -758,8 +800,11 @@
       <c r="G14">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -781,8 +826,11 @@
       <c r="G15">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -804,8 +852,11 @@
       <c r="G16">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -827,8 +878,11 @@
       <c r="G17">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -850,8 +904,11 @@
       <c r="G18">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -873,8 +930,11 @@
       <c r="G19">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -896,8 +956,11 @@
       <c r="G20">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -918,6 +981,9 @@
       </c>
       <c r="G21">
         <v>2000000</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cham cong & tinh luong
</commit_message>
<xml_diff>
--- a/KeToanTienLuong/Resources/cham_cong_form.xlsx
+++ b/KeToanTienLuong/Resources/cham_cong_form.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Số</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Tiền phạt</t>
+  </si>
+  <si>
+    <t>Số giờ tăng ca</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +443,7 @@
     <col min="7" max="7" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +468,11 @@
       <c r="H1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -491,8 +497,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -517,8 +526,11 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -543,8 +555,11 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -569,8 +584,11 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -595,8 +613,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -621,8 +642,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -647,8 +671,11 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -673,8 +700,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -699,8 +729,11 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -725,8 +758,11 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -751,8 +787,11 @@
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -777,8 +816,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -803,8 +845,11 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -829,8 +874,11 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -855,8 +903,11 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -881,8 +932,11 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -907,8 +961,11 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -933,8 +990,11 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -959,8 +1019,11 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -983,6 +1046,9 @@
         <v>2000000</v>
       </c>
       <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
         <v>0</v>
       </c>
     </row>

</xml_diff>